<commit_message>
Metadata Region (Single File) upon Excel import
</commit_message>
<xml_diff>
--- a/Templates/Facebook_v7.xlsx
+++ b/Templates/Facebook_v7.xlsx
@@ -4,33 +4,34 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
-    <sheet name="Index" sheetId="8" r:id="rId1"/>
-    <sheet name="Statements" sheetId="1" r:id="rId2"/>
-    <sheet name="Recipients" sheetId="5" r:id="rId3"/>
-    <sheet name="Services" sheetId="2" r:id="rId4"/>
-    <sheet name="PrivateData" sheetId="3" r:id="rId5"/>
-    <sheet name="Enforcements" sheetId="4" r:id="rId6"/>
-    <sheet name="Configuration Types" sheetId="6" r:id="rId7"/>
-    <sheet name="Script Data" sheetId="7" r:id="rId8"/>
+    <sheet name="Home" sheetId="9" r:id="rId1"/>
+    <sheet name="Index" sheetId="8" r:id="rId2"/>
+    <sheet name="Statements" sheetId="1" r:id="rId3"/>
+    <sheet name="Recipients" sheetId="5" r:id="rId4"/>
+    <sheet name="Services" sheetId="2" r:id="rId5"/>
+    <sheet name="PrivateData" sheetId="3" r:id="rId6"/>
+    <sheet name="Enforcements" sheetId="4" r:id="rId7"/>
+    <sheet name="Configuration Types" sheetId="6" r:id="rId8"/>
+    <sheet name="Script Data" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="enforcement_type" localSheetId="5">'Script Data'!$B$5:$F$5</definedName>
+    <definedName name="enforcement_type" localSheetId="6">'Script Data'!$B$5:$F$5</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="modality_type" localSheetId="1">'Script Data'!$B$6:$D$6</definedName>
-    <definedName name="privatedata_type" localSheetId="4">'Script Data'!$B$4:$C$4</definedName>
-    <definedName name="recipient_scope" localSheetId="2">'Script Data'!$B$2:$D$2</definedName>
-    <definedName name="recipient_type" localSheetId="2">'Script Data'!$B$3:$D$3</definedName>
-    <definedName name="statements_type" localSheetId="1">'Script Data'!$B$1:$F$1</definedName>
+    <definedName name="modality_type" localSheetId="2">'Script Data'!$B$6:$D$6</definedName>
+    <definedName name="privatedata_type" localSheetId="5">'Script Data'!$B$4:$C$4</definedName>
+    <definedName name="recipient_scope" localSheetId="3">'Script Data'!$B$2:$D$2</definedName>
+    <definedName name="recipient_type" localSheetId="3">'Script Data'!$B$3:$D$3</definedName>
+    <definedName name="statements_type" localSheetId="2">'Script Data'!$B$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="310">
   <si>
     <t>We collect the content and other information you provide when you use our Services, including when you sign up for an account, create or share, and message or communicate with others. This can include the location of a photo or the date a file was created.</t>
   </si>
@@ -963,6 +964,33 @@
   </si>
   <si>
     <t>Business Supporter Partner</t>
+  </si>
+  <si>
+    <t>Policy Name</t>
+  </si>
+  <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Organization(s)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Facebook Privacy Policy</t>
+  </si>
+  <si>
+    <t>Facebook Ireland Ltd.</t>
+  </si>
+  <si>
+    <t>7.0.0</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1257,6 +1285,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1588,10 +1618,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21">
+      <c r="A1" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="42" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="42" t="s">
+        <v>302</v>
+      </c>
+      <c r="B4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="42" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="43">
+        <v>42490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="42" t="s">
+        <v>305</v>
+      </c>
+      <c r="B7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1662,7 +1769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J92"/>
   <sheetViews>
@@ -3994,11 +4101,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4216,7 +4323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -4653,7 +4760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4812,7 +4919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4927,7 +5034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C39"/>
   <sheetViews>
@@ -5317,7 +5424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>

</xml_diff>